<commit_message>
Implemented Beta Attention on Notes Module
Implemented Beta Attention on Notes Module
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Google Drive\MCS-DS\jupyter_root\DLH\Project\dlh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B2BADD-42D2-4A0A-88B3-862CB8193EA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D3D965-AD6D-428C-8312-41CD00B66E7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17311949-DB0B-4460-9EDB-F8341AE89188}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>Notes Network</t>
   </si>
@@ -83,10 +83,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,15 +122,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,46 +450,46 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="7" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -676,24 +686,103 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>431.98700000000002</v>
+      </c>
+      <c r="E8">
+        <v>1E-3</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.67741935483870896</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.458515283842794</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.546875</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.882634375062886</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4">
+        <v>852.77</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="F9" s="4">
+        <v>10</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.87878787878787801</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.86752136752136699</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.87311827956989196</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.97723143087094499</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>450.005</v>
+      </c>
+      <c r="E10">
+        <v>1E-4</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.62944162436548201</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.48249027237353997</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.54625550660792899</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.87979205205077504</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>

</xml_diff>

<commit_message>
Hyper param experiment unbalanced
Hyper param experiment unbalanced
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Google Drive\MCS-DS\jupyter_root\DLH\Project\dlh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D330EE-86F1-41CD-A64C-88A869DFBB9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348CC77D-791C-4989-9685-1A72B76D1A24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17311949-DB0B-4460-9EDB-F8341AE89188}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>Notes Network</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Epochs</t>
   </si>
   <si>
-    <t>Precision</t>
-  </si>
-  <si>
     <t>Recall</t>
   </si>
   <si>
@@ -51,18 +48,12 @@
     <t>ROC AUC</t>
   </si>
   <si>
-    <t>Regular RNN</t>
-  </si>
-  <si>
     <t>Balanced</t>
   </si>
   <si>
     <t>Balanced / Unbalanced</t>
   </si>
   <si>
-    <t>Training Time</t>
-  </si>
-  <si>
     <t>Unbalanced</t>
   </si>
   <si>
@@ -72,18 +63,28 @@
     <t> 0.845</t>
   </si>
   <si>
-    <t>Alpha, Beta Attention</t>
-  </si>
-  <si>
-    <t>Alpha Attention</t>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Prec</t>
+  </si>
+  <si>
+    <t>α Attn</t>
+  </si>
+  <si>
+    <t>α, β Attn</t>
+  </si>
+  <si>
+    <t>RNN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,15 +103,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -118,11 +125,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39994506668294322"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -134,11 +156,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -149,6 +219,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB393238-07BA-4311-A607-FCB841AE87F3}" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="6">
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{CCA5D378-E0B4-4464-881A-19BC4501A943}" name="Notes Network" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{17D0409E-754D-4486-9EF9-1C7801E9C35B}" name="Events Network"/>
+    <tableColumn id="3" xr3:uid="{E140D059-8456-4587-9C7C-F3775C0110D0}" name="Balanced / Unbalanced"/>
+    <tableColumn id="4" xr3:uid="{DBA15C69-D6C3-4E6F-BCAA-AE18D5742B15}" name="Time" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{11BCDC2F-698A-4623-B021-99C63F38BA1A}" name="LR"/>
+    <tableColumn id="6" xr3:uid="{772E5B43-B3A2-45B0-B3F2-0083E142C1F2}" name="Epochs"/>
+    <tableColumn id="7" xr3:uid="{84287D0D-36A7-424E-8607-FA9702C40DD9}" name="Prec" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{FEA32C8A-DEBC-44A7-BD41-4237B9474BFB}" name="Recall" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{373DEF38-9C82-470C-88F8-0D81DD29B991}" name="F1" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{54A57B0D-485B-4B08-A790-115B0DF1B95A}" name="ROC AUC" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,32 +536,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8FA81D-6959-4E4F-8453-7C4184C21A78}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="7" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -482,36 +576,39 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="D2" s="7">
+        <f>D4*0.9</f>
+        <v>286.65000000000003</v>
+      </c>
       <c r="E2" s="6">
         <v>1E-3</v>
       </c>
       <c r="F2" s="6">
         <v>10</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="10">
         <v>0.62690000000000001</v>
       </c>
       <c r="H2" s="6">
@@ -524,24 +621,27 @@
         <v>0.871</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="D3" s="7">
+        <f>D5*0.9</f>
+        <v>566.93700000000001</v>
+      </c>
       <c r="E3" s="6">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="F3" s="6">
         <v>10</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="10">
         <v>0.17799999999999999</v>
       </c>
       <c r="H3" s="6">
@@ -554,17 +654,17 @@
         <v>0.76500000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8">
         <v>318.5</v>
       </c>
       <c r="E4">
@@ -573,7 +673,7 @@
       <c r="F4">
         <v>10</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="11">
         <v>0.69021739130434701</v>
       </c>
       <c r="H4" s="2">
@@ -586,17 +686,17 @@
         <v>0.87942744174387599</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8">
         <v>629.92999999999995</v>
       </c>
       <c r="E5">
@@ -605,7 +705,7 @@
       <c r="F5">
         <v>10</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="11">
         <v>0.39121756487025899</v>
       </c>
       <c r="H5" s="2">
@@ -618,17 +718,17 @@
         <v>0.89613730514943601</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8">
         <v>279.23</v>
       </c>
       <c r="E6">
@@ -637,7 +737,7 @@
       <c r="F6">
         <v>10</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="11">
         <v>0.72799999999999998</v>
       </c>
       <c r="H6" s="2">
@@ -647,20 +747,20 @@
         <v>0.41699999999999998</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8">
         <v>610.52</v>
       </c>
       <c r="E7">
@@ -669,7 +769,7 @@
       <c r="F7">
         <v>10</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="11">
         <v>0.84699999999999998</v>
       </c>
       <c r="H7" s="2">
@@ -679,20 +779,20 @@
         <v>0.86099999999999999</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8">
         <v>400.16</v>
       </c>
       <c r="E8">
@@ -701,7 +801,7 @@
       <c r="F8">
         <v>10</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="11">
         <v>0.73799999999999999</v>
       </c>
       <c r="H8" s="2">
@@ -714,17 +814,17 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="D9" s="8">
         <v>741.47</v>
       </c>
       <c r="E9">
@@ -733,7 +833,7 @@
       <c r="F9">
         <v>10</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="11">
         <v>0.877</v>
       </c>
       <c r="H9" s="2">
@@ -746,17 +846,17 @@
         <v>0.97599999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8">
         <v>431.98700000000002</v>
       </c>
       <c r="E10">
@@ -765,7 +865,7 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="11">
         <v>0.66081871345029197</v>
       </c>
       <c r="H10" s="2">
@@ -778,17 +878,17 @@
         <v>0.90801600776133795</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4">
+        <v>7</v>
+      </c>
+      <c r="D11" s="9">
         <v>852.77</v>
       </c>
       <c r="E11" s="4">
@@ -797,7 +897,7 @@
       <c r="F11" s="4">
         <v>10</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="12">
         <v>0.87878787878787801</v>
       </c>
       <c r="H11" s="5">
@@ -810,58 +910,38 @@
         <v>0.97723143087094499</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12">
-        <v>450.005</v>
-      </c>
-      <c r="E12">
-        <v>1E-4</v>
-      </c>
-      <c r="F12">
-        <v>10</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.62944162436548201</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.48249027237353997</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.54625550660792899</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.87979205205077504</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="14"/>
+      <c r="K13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="15"/>
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -933,14 +1013,11 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of experiment with essential features
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Google Drive\MCS-DS\jupyter_root\DLH\Project\dlh-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnoya\OneDrive\University of Illinois\CS 598 - Deep Learning for Healthcare\Project\repository\dlh-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348CC77D-791C-4989-9685-1A72B76D1A24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193FAEE5-547E-4823-BAB6-61D9A75C113B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17311949-DB0B-4460-9EDB-F8341AE89188}"/>
+    <workbookView xWindow="11640" yWindow="0" windowWidth="17280" windowHeight="9105" xr2:uid="{17311949-DB0B-4460-9EDB-F8341AE89188}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>Notes Network</t>
   </si>
@@ -76,6 +85,12 @@
   </si>
   <si>
     <t>RNN</t>
+  </si>
+  <si>
+    <t>Reduced number of features (8 out of 20).  Selection based on beta attention weights.</t>
+  </si>
+  <si>
+    <t>Observations</t>
   </si>
 </sst>
 </file>
@@ -84,7 +99,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -144,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -159,21 +174,22 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -183,6 +199,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -222,25 +241,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB393238-07BA-4311-A607-FCB841AE87F3}" name="Table2" displayName="Table2" ref="A1:J11" totalsRowShown="0" headerRowDxfId="6">
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{CCA5D378-E0B4-4464-881A-19BC4501A943}" name="Notes Network" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB393238-07BA-4311-A607-FCB841AE87F3}" name="Table2" displayName="Table2" ref="A1:K12" totalsRowShown="0" headerRowDxfId="7">
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{CCA5D378-E0B4-4464-881A-19BC4501A943}" name="Notes Network" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{17D0409E-754D-4486-9EF9-1C7801E9C35B}" name="Events Network"/>
     <tableColumn id="3" xr3:uid="{E140D059-8456-4587-9C7C-F3775C0110D0}" name="Balanced / Unbalanced"/>
-    <tableColumn id="4" xr3:uid="{DBA15C69-D6C3-4E6F-BCAA-AE18D5742B15}" name="Time" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{DBA15C69-D6C3-4E6F-BCAA-AE18D5742B15}" name="Time" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{11BCDC2F-698A-4623-B021-99C63F38BA1A}" name="LR"/>
     <tableColumn id="6" xr3:uid="{772E5B43-B3A2-45B0-B3F2-0083E142C1F2}" name="Epochs"/>
-    <tableColumn id="7" xr3:uid="{84287D0D-36A7-424E-8607-FA9702C40DD9}" name="Prec" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{FEA32C8A-DEBC-44A7-BD41-4237B9474BFB}" name="Recall" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{373DEF38-9C82-470C-88F8-0D81DD29B991}" name="F1" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{54A57B0D-485B-4B08-A790-115B0DF1B95A}" name="ROC AUC" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{84287D0D-36A7-424E-8607-FA9702C40DD9}" name="Prec" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{FEA32C8A-DEBC-44A7-BD41-4237B9474BFB}" name="Recall" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{373DEF38-9C82-470C-88F8-0D81DD29B991}" name="F1" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{54A57B0D-485B-4B08-A790-115B0DF1B95A}" name="ROC AUC" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{281F2AB2-0523-470D-A32F-934950603C91}" name="Observations" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -536,24 +556,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F8FA81D-6959-4E4F-8453-7C4184C21A78}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J12" sqref="D12:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" customWidth="1"/>
     <col min="9" max="9" width="6.42578125" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="11" max="11" width="78.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -587,6 +607,9 @@
       <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -620,6 +643,7 @@
       <c r="J2" s="6">
         <v>0.871</v>
       </c>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -653,6 +677,7 @@
       <c r="J3" s="6">
         <v>0.76500000000000001</v>
       </c>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -685,6 +710,7 @@
       <c r="J4" s="2">
         <v>0.87942744174387599</v>
       </c>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -717,6 +743,7 @@
       <c r="J5" s="2">
         <v>0.89613730514943601</v>
       </c>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -749,6 +776,7 @@
       <c r="J6" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -781,6 +809,7 @@
       <c r="J7" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -813,6 +842,7 @@
       <c r="J8" s="2">
         <v>0.879</v>
       </c>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -845,6 +875,7 @@
       <c r="J9" s="2">
         <v>0.97599999999999998</v>
       </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -877,6 +908,7 @@
       <c r="J10" s="2">
         <v>0.90801600776133795</v>
       </c>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -909,37 +941,67 @@
       <c r="J11" s="5">
         <v>0.97723143087094499</v>
       </c>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="7">
+        <v>7964</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="F12" s="6">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.62260000000000004</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0.38969999999999999</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.47939999999999999</v>
+      </c>
+      <c r="J12" s="16">
+        <v>0.86650000000000005</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="14"/>
-      <c r="K13" t="s">
-        <v>9</v>
-      </c>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="15"/>
+      <c r="J14" s="14"/>
       <c r="K14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="J15" s="15"/>
+      <c r="K15" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
@@ -1012,6 +1074,12 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>